<commit_message>
Most recent updates 5-03-2024
</commit_message>
<xml_diff>
--- a/simulations/function_requirements/ip_facilities_info.xlsx
+++ b/simulations/function_requirements/ip_facilities_info.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,7 +428,7 @@
         <v>236.1769911504425</v>
       </c>
       <c r="H2">
-        <v>0.519290615210646</v>
+        <v>0.5275666176396232</v>
       </c>
     </row>
     <row r="3">
@@ -460,7 +460,7 @@
         <v>236.7091703056768</v>
       </c>
       <c r="H3">
-        <v>1.065373770927743</v>
+        <v>1.111453171863835</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         <v>236.1769911504425</v>
       </c>
       <c r="H4">
-        <v>0.4715638484582704</v>
+        <v>0.4893562365297635</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>132.0774193548387</v>
       </c>
       <c r="H5">
-        <v>1.909363028241947</v>
+        <v>1.991946537346263</v>
       </c>
     </row>
     <row r="6">
@@ -556,7 +556,7 @@
         <v>188.5888324873096</v>
       </c>
       <c r="H6">
-        <v>1.337214606271589</v>
+        <v>1.39505162991666</v>
       </c>
     </row>
     <row r="7">
@@ -588,7 +588,7 @@
         <v>186.6810810810811</v>
       </c>
       <c r="H7">
-        <v>1.350880013771752</v>
+        <v>1.409308091756941</v>
       </c>
     </row>
     <row r="8">
@@ -620,7 +620,7 @@
         <v>300.6760563380282</v>
       </c>
       <c r="H8">
-        <v>1.060390922508506</v>
+        <v>1.137786789283417</v>
       </c>
     </row>
     <row r="9">
@@ -652,7 +652,7 @@
         <v>115.7363896848138</v>
       </c>
       <c r="H9">
-        <v>0.9622948423352381</v>
+        <v>0.9986028064211235</v>
       </c>
     </row>
     <row r="10">
@@ -684,7 +684,7 @@
         <v>115.7363896848138</v>
       </c>
       <c r="H10">
-        <v>1.059688274077943</v>
+        <v>1.076576664650283</v>
       </c>
     </row>
     <row r="11">
@@ -716,7 +716,7 @@
         <v>165.8057142857143</v>
       </c>
       <c r="H11">
-        <v>0.7396879870000931</v>
+        <v>0.7514764911590116</v>
       </c>
     </row>
     <row r="12">
@@ -748,7 +748,7 @@
         <v>245.830243902439</v>
       </c>
       <c r="H12">
-        <v>1.025845060308441</v>
+        <v>1.070214770847774</v>
       </c>
     </row>
     <row r="13">
@@ -780,7 +780,7 @@
         <v>165.8057142857143</v>
       </c>
       <c r="H13">
-        <v>0.6717050214100692</v>
+        <v>0.6970488565016943</v>
       </c>
     </row>
     <row r="14">
@@ -812,7 +812,7 @@
         <v>245.830243902439</v>
       </c>
       <c r="H14">
-        <v>1.296968817567601</v>
+        <v>1.391632043822133</v>
       </c>
     </row>
     <row r="15">
@@ -844,7 +844,7 @@
         <v>263.8890600924499</v>
       </c>
       <c r="H15">
-        <v>0.9556430315579857</v>
+        <v>0.9969763735310998</v>
       </c>
     </row>
     <row r="16">
@@ -876,7 +876,7 @@
         <v>320.7197802197802</v>
       </c>
       <c r="H16">
-        <v>0.7863055443880697</v>
+        <v>0.8203147244775868</v>
       </c>
     </row>
     <row r="17">
@@ -908,7 +908,7 @@
         <v>165.294964028777</v>
       </c>
       <c r="H17">
-        <v>0.7419735728413409</v>
+        <v>0.753798502680639</v>
       </c>
     </row>
     <row r="18">
@@ -940,7 +940,7 @@
         <v>165.294964028777</v>
       </c>
       <c r="H18">
-        <v>1.525658950733868</v>
+        <v>1.591646543446408</v>
       </c>
     </row>
     <row r="19">
@@ -972,7 +972,7 @@
         <v>165.294964028777</v>
       </c>
       <c r="H19">
-        <v>1.928880063768875</v>
+        <v>2.069665260314198</v>
       </c>
     </row>
     <row r="20">
@@ -1004,7 +1004,7 @@
         <v>162.8823529411765</v>
       </c>
       <c r="H20">
-        <v>0.7529636748150647</v>
+        <v>0.7649637553464128</v>
       </c>
     </row>
     <row r="21">
@@ -1036,7 +1036,7 @@
         <v>162.8823529411765</v>
       </c>
       <c r="H21">
-        <v>1.548256989342549</v>
+        <v>1.615221989336772</v>
       </c>
     </row>
     <row r="22">
@@ -1068,7 +1068,7 @@
         <v>162.8823529411765</v>
       </c>
       <c r="H22">
-        <v>1.957450607750278</v>
+        <v>2.100321112617971</v>
       </c>
     </row>
     <row r="23">
@@ -1100,7 +1100,7 @@
         <v>284.7272727272727</v>
       </c>
       <c r="H23">
-        <v>1.119787920920023</v>
+        <v>1.201519058846645</v>
       </c>
     </row>
     <row r="24">
@@ -1132,7 +1132,7 @@
         <v>197.8496583143508</v>
       </c>
       <c r="H24">
-        <v>1.274623082649238</v>
+        <v>1.329752906257196</v>
       </c>
     </row>
     <row r="25">
@@ -1164,7 +1164,7 @@
         <v>254.6341463414634</v>
       </c>
       <c r="H25">
-        <v>0.4816498368158636</v>
+        <v>0.4893259532382404</v>
       </c>
     </row>
     <row r="26">
@@ -1196,7 +1196,7 @@
         <v>241.1391705069124</v>
       </c>
       <c r="H26">
-        <v>1.04580164579486</v>
+        <v>1.091034515845942</v>
       </c>
     </row>
     <row r="27">
@@ -1228,7 +1228,7 @@
         <v>254.6341463414634</v>
       </c>
       <c r="H27">
-        <v>0.4373825445816187</v>
+        <v>0.4538852514670935</v>
       </c>
     </row>
     <row r="28">
@@ -1260,7 +1260,7 @@
         <v>241.1391705069124</v>
       </c>
       <c r="H28">
-        <v>1.322199790628215</v>
+        <v>1.418704576432297</v>
       </c>
     </row>
     <row r="29">
@@ -1292,7 +1292,7 @@
         <v>149.625</v>
       </c>
       <c r="H29">
-        <v>1.685438538892139</v>
+        <v>1.758336896544703</v>
       </c>
     </row>
     <row r="30">
@@ -1324,7 +1324,7 @@
         <v>260.0275862068966</v>
       </c>
       <c r="H30">
-        <v>0.9698345666335605</v>
+        <v>1.011781718944878</v>
       </c>
     </row>
     <row r="31">
@@ -1484,7 +1484,7 @@
         <v>565.5652173913044</v>
       </c>
       <c r="H35">
-        <v>0.5637442879304679</v>
+        <v>0.604890884791715</v>
       </c>
     </row>
     <row r="36">
@@ -1516,7 +1516,7 @@
         <v>203.8140221402214</v>
       </c>
       <c r="H36">
-        <v>1.237322823687946</v>
+        <v>1.290839341586115</v>
       </c>
     </row>
     <row r="37">
@@ -1548,7 +1548,7 @@
         <v>203.8140221402214</v>
       </c>
       <c r="H37">
-        <v>1.564338691756681</v>
+        <v>1.678516724035213</v>
       </c>
     </row>
     <row r="38">
@@ -1580,7 +1580,7 @@
         <v>418.4810126582278</v>
       </c>
       <c r="H38">
-        <v>0.761884413180992</v>
+        <v>0.8174928716171911</v>
       </c>
     </row>
     <row r="39">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>New Ulm Adolescent/Adult</t>
+          <t>New Ulm Adult</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1602,17 +1602,17 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Adolescent</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F39">
-        <v>0.1159984429739198</v>
+        <v>0.1711659965537048</v>
       </c>
       <c r="G39">
         <v>201.503355704698</v>
       </c>
       <c r="H39">
-        <v>0.6086474074052016</v>
+        <v>1.305641572198231</v>
       </c>
     </row>
     <row r="40">
@@ -1620,16 +1620,16 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>New Ulm Adolescent/Adult</t>
+          <t>North Memorial Adult</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>New Ulm Medical Center</t>
+          <t>North Memorial Health Hospital</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1638,13 +1638,13 @@
         </is>
       </c>
       <c r="F40">
-        <v>0.1159984429739198</v>
+        <v>0.2107983917288914</v>
       </c>
       <c r="G40">
-        <v>201.503355704698</v>
+        <v>333.1226158038147</v>
       </c>
       <c r="H40">
-        <v>1.251511373097479</v>
+        <v>0.7897727313129739</v>
       </c>
     </row>
     <row r="41">
@@ -1652,16 +1652,16 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>North Memorial Adult</t>
+          <t>Owatonna Adult</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>North Memorial Health Hospital</t>
+          <t>Owatonna Hospital</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1670,13 +1670,13 @@
         </is>
       </c>
       <c r="F41">
-        <v>0.2107983917288914</v>
+        <v>0.1728891441700172</v>
       </c>
       <c r="G41">
-        <v>333.1226158038147</v>
+        <v>217.6744186046512</v>
       </c>
       <c r="H41">
-        <v>0.7570297824818187</v>
+        <v>1.208645277805187</v>
       </c>
     </row>
     <row r="42">
@@ -1684,31 +1684,31 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Owatonna Adult</t>
+          <t>PrairieCare Pediatric/Adolescent</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Owatonna Hospital</t>
+          <t>PrairieCare</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Adolescent</t>
         </is>
       </c>
       <c r="F42">
-        <v>0.1728891441700172</v>
+        <v>3.429611650485437</v>
       </c>
       <c r="G42">
-        <v>217.6744186046512</v>
+        <v>184.5859872611465</v>
       </c>
       <c r="H42">
-        <v>1.158536418740883</v>
+        <v>0.6750192592315432</v>
       </c>
     </row>
     <row r="43">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Adolescent</t>
+          <t>Child</t>
         </is>
       </c>
       <c r="F43">
@@ -1740,7 +1740,7 @@
         <v>184.5859872611465</v>
       </c>
       <c r="H43">
-        <v>0.6644301490751785</v>
+        <v>0.6261292379729364</v>
       </c>
     </row>
     <row r="44">
@@ -1748,31 +1748,31 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>PrairieCare Pediatric/Adolescent</t>
+          <t>Regina Geriatric</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PrairieCare</t>
+          <t>Regina Hospital</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Child</t>
+          <t>Geriatric</t>
         </is>
       </c>
       <c r="F44">
-        <v>3.429611650485437</v>
+        <v>0.02067777139574957</v>
       </c>
       <c r="G44">
-        <v>184.5859872611465</v>
+        <v>572</v>
       </c>
       <c r="H44">
-        <v>0.6033639525769156</v>
+        <v>0.5980860922294489</v>
       </c>
     </row>
     <row r="45">
@@ -1780,31 +1780,31 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Regina Geriatric</t>
+          <t>Regions Adult</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Regina Hospital</t>
+          <t>Regions Hospital</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Geriatric</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F45">
-        <v>0.02067777139574957</v>
+        <v>1.136128661688685</v>
       </c>
       <c r="G45">
-        <v>572</v>
+        <v>267.360970677452</v>
       </c>
       <c r="H45">
-        <v>0.5574023789449322</v>
+        <v>0.9840297836997983</v>
       </c>
     </row>
     <row r="46">
@@ -1812,31 +1812,31 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Regions Adult</t>
+          <t>Ridgeview Geriatric</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Regions Hospital</t>
+          <t>Ridgeview Medical Center</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Geriatric</t>
         </is>
       </c>
       <c r="F46">
-        <v>1.136128661688685</v>
+        <v>0.007466973004020678</v>
       </c>
       <c r="G46">
-        <v>267.360970677452</v>
+        <v>164.3076923076923</v>
       </c>
       <c r="H46">
-        <v>0.9432331904793028</v>
+        <v>2.082101208716377</v>
       </c>
     </row>
     <row r="47">
@@ -1844,31 +1844,31 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ridgeview Geriatric</t>
+          <t>St Jospephs Adult/Geriatric</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Ridgeview Medical Center</t>
+          <t>Saint Joseph's Hospital</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Geriatric</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F47">
-        <v>0.007466973004020678</v>
+        <v>0.7375071797817346</v>
       </c>
       <c r="G47">
-        <v>164.3076923076923</v>
+        <v>262.6542056074766</v>
       </c>
       <c r="H47">
-        <v>1.940470079510541</v>
+        <v>1.001663603813287</v>
       </c>
     </row>
     <row r="48">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Geriatric</t>
         </is>
       </c>
       <c r="F48">
@@ -1900,7 +1900,7 @@
         <v>262.6542056074766</v>
       </c>
       <c r="H48">
-        <v>0.9601359353773764</v>
+        <v>1.302492925875719</v>
       </c>
     </row>
     <row r="49">
@@ -1908,31 +1908,31 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>St Jospephs Adult/Geriatric</t>
+          <t>Sanford Behavioral Adolescent/Adult/Geriatric</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Saint Joseph's Hospital</t>
+          <t>Sanford Behavioral Health Center</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Geriatric</t>
+          <t>Adolescent</t>
         </is>
       </c>
       <c r="F49">
-        <v>0.7375071797817346</v>
+        <v>0.08836123005060335</v>
       </c>
       <c r="G49">
-        <v>262.6542056074766</v>
+        <v>145.057268722467</v>
       </c>
       <c r="H49">
-        <v>1.213893225197325</v>
+        <v>0.8589648590718558</v>
       </c>
     </row>
     <row r="50">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Adolescent</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F50">
@@ -1964,7 +1964,7 @@
         <v>145.057268722467</v>
       </c>
       <c r="H50">
-        <v>0.8454901716629176</v>
+        <v>1.813705445184304</v>
       </c>
     </row>
     <row r="51">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Geriatric</t>
         </is>
       </c>
       <c r="F51">
@@ -1996,7 +1996,7 @@
         <v>145.057268722467</v>
       </c>
       <c r="H51">
-        <v>1.738511579617776</v>
+        <v>2.358415043714789</v>
       </c>
     </row>
     <row r="52">
@@ -2004,31 +2004,31 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Sanford Behavioral Adolescent/Adult/Geriatric</t>
+          <t>St. Cloud Adolescent/Adult</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Sanford Behavioral Health Center</t>
+          <t>St. Cloud Hospital</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Geriatric</t>
+          <t>Adolescent</t>
         </is>
       </c>
       <c r="F52">
-        <v>0.08836123005060335</v>
+        <v>0.3386531724406384</v>
       </c>
       <c r="G52">
-        <v>145.057268722467</v>
+        <v>180</v>
       </c>
       <c r="H52">
-        <v>2.197988170910039</v>
+        <v>0.692217202141901</v>
       </c>
     </row>
     <row r="53">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Adolescent</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F53">
@@ -2060,7 +2060,7 @@
         <v>180</v>
       </c>
       <c r="H53">
-        <v>0.6813583057395143</v>
+        <v>1.461617545252784</v>
       </c>
     </row>
     <row r="54">
@@ -2068,16 +2068,16 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>St. Cloud Adolescent/Adult</t>
+          <t>Essentia St. Josephs Adult</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>St. Cloud Hospital</t>
+          <t>St. Joseph's Medical Center</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2086,13 +2086,13 @@
         </is>
       </c>
       <c r="F54">
-        <v>0.3386531724406384</v>
+        <v>0.2056289488799541</v>
       </c>
       <c r="G54">
-        <v>180</v>
+        <v>124.6256983240224</v>
       </c>
       <c r="H54">
-        <v>1.401020785454091</v>
+        <v>2.111050623455474</v>
       </c>
     </row>
     <row r="55">
@@ -2104,12 +2104,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Essentia St. Josephs Adult</t>
+          <t>St Lukes Adult</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>St. Joseph's Medical Center</t>
+          <t>St. Luke's Hospital</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2118,13 +2118,13 @@
         </is>
       </c>
       <c r="F55">
-        <v>0.2056289488799541</v>
+        <v>0.2952326249282022</v>
       </c>
       <c r="G55">
-        <v>124.6256983240224</v>
+        <v>268.0622568093385</v>
       </c>
       <c r="H55">
-        <v>2.023529214063601</v>
+        <v>0.9814554323200634</v>
       </c>
     </row>
     <row r="56">
@@ -2132,31 +2132,31 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>St Lukes Adult</t>
+          <t>United Adolescent</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>St. Luke's Hospital</t>
+          <t>United Hospital</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Adolescent</t>
         </is>
       </c>
       <c r="F56">
-        <v>0.2952326249282022</v>
+        <v>0.299757281553398</v>
       </c>
       <c r="G56">
-        <v>268.0622568093385</v>
+        <v>258.6558704453441</v>
       </c>
       <c r="H56">
-        <v>0.9407655683549068</v>
+        <v>0.4817176434890577</v>
       </c>
     </row>
     <row r="57">
@@ -2164,11 +2164,11 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>United Adolescent</t>
+          <t>United Adult/Geriatric</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2178,17 +2178,17 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Adolescent</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F57">
-        <v>0.299757281553398</v>
+        <v>0.3739230327398047</v>
       </c>
       <c r="G57">
-        <v>258.6558704453441</v>
+        <v>240.073732718894</v>
       </c>
       <c r="H57">
-        <v>0.4741608795576447</v>
+        <v>1.095876484136474</v>
       </c>
     </row>
     <row r="58">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>Geriatric</t>
         </is>
       </c>
       <c r="F58">
@@ -2220,7 +2220,7 @@
         <v>240.073732718894</v>
       </c>
       <c r="H58">
-        <v>1.050442872386302</v>
+        <v>1.425000731570334</v>
       </c>
     </row>
     <row r="59">
@@ -2228,63 +2228,31 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>United Adult/Geriatric</t>
+          <t>Winnona Adult</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>United Hospital</t>
+          <t>Winona Health Services</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Geriatric</t>
+          <t>Adult</t>
         </is>
       </c>
       <c r="F59">
-        <v>0.3739230327398047</v>
+        <v>0.01033888569787478</v>
       </c>
       <c r="G59">
-        <v>240.073732718894</v>
+        <v>169.3333333333333</v>
       </c>
       <c r="H59">
-        <v>1.328067661320653</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>10</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Winnona Adult</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Winona Health Services</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Adult</t>
-        </is>
-      </c>
-      <c r="F60">
-        <v>0.01033888569787478</v>
-      </c>
-      <c r="G60">
-        <v>169.3333333333333</v>
-      </c>
-      <c r="H60">
-        <v>1.48927406327797</v>
+        <v>1.553687941804141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>